<commit_message>
Se modifica readme y se agrega captura
</commit_message>
<xml_diff>
--- a/Pruebas Proyecto Python CH.xlsx
+++ b/Pruebas Proyecto Python CH.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alef2\OneDrive\Escritorio\Proyecto Final Coder House\z TercerapreentregaFernandezAlejandro-master\TercerapreentregaF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alef2\OneDrive\Escritorio\Proyecto Final Coder House\z TercerapreentregaFernandezAlejandro-master\TercerapreentregaF - 1 Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED0D49A-E021-4887-9BEE-1AF23AC5D947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7331DC7A-9C46-4B4C-A501-ABAEC625BCE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12000" yWindow="0" windowWidth="12000" windowHeight="12900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="51">
   <si>
     <t>Nombre del Proyecto</t>
   </si>
@@ -78,97 +78,106 @@
     <t>Si</t>
   </si>
   <si>
-    <t>Johannes Pérez</t>
-  </si>
-  <si>
-    <t>Chrome</t>
-  </si>
-  <si>
-    <t>Version 101.0.4951.67</t>
-  </si>
-  <si>
-    <t>Página de Venta y Permuta de Instrumentos Musicales</t>
-  </si>
-  <si>
-    <t>Buenos Aires, Argentina</t>
-  </si>
-  <si>
     <t>Registro de Usuario</t>
   </si>
   <si>
     <t>Todos van a una página o sección distinta</t>
   </si>
   <si>
-    <t>Carga de Instrumento Musicales</t>
-  </si>
-  <si>
-    <t>Carga de Comentario</t>
-  </si>
-  <si>
-    <t>Edición de Instrumento</t>
-  </si>
-  <si>
-    <t>Nuevo instrumento visible dependiendo de la categoria del instrumento (ejemplo:guitarra). Una vez el instrumento es ingresado a la BD el usuario es dirigido al inicio (El ingreso del instrumento musical se realiza en el formulario disponible en el inicio de la página web</t>
-  </si>
-  <si>
-    <t>Eliminación de Instrumento Musical</t>
-  </si>
-  <si>
-    <t>Edición de Perfil de Usuario</t>
-  </si>
-  <si>
-    <t>Independientemente de la página que el usuario se encuentre, al hacer click en perfil, el usuario será dirigo a editar su perfil en el cual podrá cambiar los datos a excepción del password, el cual hay un vinculo que lo lleva a una página para el cambio de dicho password, tanto al hacer click en guardar en editar perfil como cambiar la contraseña, en ambos casos el usuario será redigido a lá página de inicio</t>
-  </si>
-  <si>
     <t>Logout</t>
   </si>
   <si>
-    <t>Al hacer click en logout, el usuario automaticamente estará fuera de su sesión</t>
-  </si>
-  <si>
     <t>Login Requerido</t>
   </si>
   <si>
-    <t>Cuando el usuario no esté autenticado, este será solicitado que inicie sesión para visitar las distintas páginas. La única sección que no es requerido el inicio de sesión es la sección "Conóceme"</t>
-  </si>
-  <si>
     <t>Hacer click a los links (a href)</t>
   </si>
   <si>
-    <t>Una vez que se carga el comentario en el detalle del instrumento, el usuario es dirigido al inicio</t>
-  </si>
-  <si>
-    <t>Cuando se edita (icono de lápiz en al lado de la imagen del instrumento) la información de un instrumento musical (ejemplo bajo) el usuario es dirigido al detalle del instrumento, una vez que guarda los cambios, el usuario es redirigido a la lista de instrumentos musicales que se encontraba anteriormente (ejemplo: lista de bajos)</t>
-  </si>
-  <si>
-    <t>Dentro del listado de instrumentos(ejemplo teclados) cuando el usuario hace click en el icono de basura al lado de la imagen del instrumento, el usuario será digido a una página de eliminación del instrumento, al hacer click en eliminar, dicho instrumento será removido de la base de datos y el usuario sera redirigido a la página del listado que se encontraba anteriormente (ejemplo teclados)</t>
-  </si>
-  <si>
-    <t>Proyecto Final Coder House Python (Comisión 27615)</t>
-  </si>
-  <si>
-    <t>Se actualiza el avatar del usuario en una segunda instancia</t>
-  </si>
-  <si>
     <t>Un solo avatar en el modelo de avatares</t>
   </si>
   <si>
     <t>Se comprobó en el panel admin que un solo avatar estaba relacionado a su usuario</t>
   </si>
   <si>
-    <t>El nombre apellido, etc se modificaron y se actualizaron</t>
-  </si>
-  <si>
-    <t>Se actualizaron todos menos la profesion</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
     <t>Sí</t>
   </si>
   <si>
-    <t>Modificacion de Profesor</t>
+    <t>Alejandro Fernandez</t>
+  </si>
+  <si>
+    <t>Proyecto Final Coder House Python (Comisión 43865)</t>
+  </si>
+  <si>
+    <t>Opera</t>
+  </si>
+  <si>
+    <t>Version 101.0.4843.33</t>
+  </si>
+  <si>
+    <t>Página Web Centro de Salud</t>
+  </si>
+  <si>
+    <t>El nombre de la  especialidad,  el nombre del doctor,  se modificaron y se actualizaron</t>
+  </si>
+  <si>
+    <t>Modificación de Especialidad</t>
+  </si>
+  <si>
+    <t>Sacar Turno en Turnos</t>
+  </si>
+  <si>
+    <t>Lista de  especialidad,  nombre y dni,  se modificaron y se actualizaron</t>
+  </si>
+  <si>
+    <t>Se actualizaron todos</t>
+  </si>
+  <si>
+    <t>Buscador de Especialidades</t>
+  </si>
+  <si>
+    <t>Cambio comportamiento boton Login-Register a logout</t>
+  </si>
+  <si>
+    <t>Cambio en la barra del menu</t>
+  </si>
+  <si>
+    <t>se actualizaron los button register login logout</t>
+  </si>
+  <si>
+    <t>buscar y listar con el nombre del doctor, en caso de no encontrar resultado, enviar aviso</t>
+  </si>
+  <si>
+    <t>Se comprobó que la especialidad con el nombre del doctor fue encontrada, aviso de no encontrar resultado se visualizo perfectamente</t>
+  </si>
+  <si>
+    <t>Al hacer click en salir, el usuario automaticamente estará fuera de su sesión</t>
+  </si>
+  <si>
+    <t>Cuando el usuario no esté autenticado, este será solicitado que inicie sesión para ver o sacar turnos, idem para Mi perfil o editar Especialidades</t>
+  </si>
+  <si>
+    <t>Cuando el usuario no esté autenticado, este será solicitado que inicie sesión para ver o sacar turnos, idem para Mi Perfil o editar Especialidades</t>
+  </si>
+  <si>
+    <t>Blog</t>
+  </si>
+  <si>
+    <t>Se comprobó que la creacion de post para el blog  desde el admin se visualizaron correctamente</t>
+  </si>
+  <si>
+    <t>Córdoba, Argentina</t>
+  </si>
+  <si>
+    <t>Se actualiza el avatar del usuario en una segunda instancia y en la seccion mi perfil</t>
+  </si>
+  <si>
+    <t>Lista de post en blog con fecha y categoria y al hacer click ampliar la info</t>
+  </si>
+  <si>
+    <t>Se actualizaron todos menos la CAR en detail</t>
   </si>
 </sst>
 </file>
@@ -556,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,14 +586,14 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="F1" s="6"/>
     </row>
@@ -600,7 +609,7 @@
         <v>12</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="F2" s="6"/>
     </row>
@@ -609,14 +618,14 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F3" s="6"/>
     </row>
@@ -625,14 +634,14 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="F4" s="6"/>
     </row>
@@ -661,7 +670,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="4">
-        <v>44711</v>
+        <v>45154</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>14</v>
@@ -681,10 +690,10 @@
         <v>2</v>
       </c>
       <c r="B8" s="4">
-        <v>44711</v>
+        <v>45154</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>15</v>
@@ -696,153 +705,161 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>3</v>
+      </c>
+      <c r="B9" s="4">
+        <v>45154</v>
+      </c>
       <c r="C9" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>41</v>
+        <v>37</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
+      <c r="A10" s="3">
+        <v>4</v>
+      </c>
+      <c r="B10" s="4">
+        <v>45154</v>
+      </c>
       <c r="C10" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B11" s="4">
-        <v>44711</v>
-      </c>
-      <c r="C11" s="3" t="s">
+        <v>45154</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>6</v>
+      </c>
+      <c r="B12" s="4">
+        <v>45154</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>7</v>
+      </c>
+      <c r="B13" s="4">
+        <v>45154</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="120" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>4</v>
-      </c>
-      <c r="B12" s="4">
-        <v>44711</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
-        <v>5</v>
-      </c>
-      <c r="B13" s="4">
-        <v>44711</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>36</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B14" s="4">
-        <v>44711</v>
+        <v>45154</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="180" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B15" s="4">
-        <v>44711</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>28</v>
+        <v>45154</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B16" s="4">
-        <v>44711</v>
+        <v>45154</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>16</v>
@@ -850,43 +867,26 @@
     </row>
     <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B17" s="4">
-        <v>44711</v>
+        <v>45154</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
-        <v>10</v>
-      </c>
-      <c r="B18" s="4">
-        <v>44711</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>16</v>
-      </c>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F19" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>